<commit_message>
Styling, help, log, dll
</commit_message>
<xml_diff>
--- a/src/utils/excel-data.xlsx
+++ b/src/utils/excel-data.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Blog\Learn\App\CropID\archive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Blog\GitHub\CropID\src\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE964BC-0D6A-4FDB-9A02-238448822132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9B6DD8-077E-42B4-85C6-E2836FB4C06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="847" firstSheet="3" activeTab="14" xr2:uid="{096C9FAE-DC65-42E7-9532-324409CBB1AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="847" firstSheet="1" activeTab="1" xr2:uid="{096C9FAE-DC65-42E7-9532-324409CBB1AD}"/>
   </bookViews>
   <sheets>
     <sheet name="TEST" sheetId="15" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="17" r:id="rId2"/>
+    <sheet name="Sheet 1" sheetId="17" r:id="rId2"/>
     <sheet name="AVS-RAKRAL" sheetId="1" r:id="rId3"/>
     <sheet name="AVS-F" sheetId="8" r:id="rId4"/>
     <sheet name="AVS-RPT" sheetId="16" r:id="rId5"/>
@@ -1918,7 +1918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52CA380A-2E51-43B1-B44A-0B233E19F869}">
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -3181,8 +3181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33ED886F-F38A-4300-8F5D-73DF309E02E9}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>